<commit_message>
successfully implemented multiple updates to multiple dataframes
</commit_message>
<xml_diff>
--- a/bill_russell_and_wilt_chamberlain_per_game_avgs_merged.xlsx
+++ b/bill_russell_and_wilt_chamberlain_per_game_avgs_merged.xlsx
@@ -367,18 +367,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -408,13 +402,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -949,2462 +941,2294 @@
       </c>
     </row>
     <row r="2" spans="1:77">
-      <c r="A2" s="2">
+      <c r="A2">
         <v>3513</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" t="s">
         <v>77</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2">
         <v>610</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" t="s">
         <v>87</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2">
         <v>1935</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" t="s">
         <v>88</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2">
         <v>34</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2">
         <v>13</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" t="s">
         <v>89</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" t="s">
         <v>90</v>
       </c>
-      <c r="K2" s="2">
+      <c r="K2">
         <v>77</v>
       </c>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2">
+      <c r="M2">
         <v>42.7</v>
       </c>
-      <c r="N2" s="2">
+      <c r="N2">
         <v>3.6</v>
       </c>
-      <c r="O2" s="2">
+      <c r="O2">
         <v>8.4</v>
       </c>
-      <c r="P2" s="2">
+      <c r="P2">
         <v>0.433</v>
       </c>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2">
+      <c r="T2">
         <v>3.6</v>
       </c>
-      <c r="U2" s="2">
+      <c r="U2">
         <v>8.4</v>
       </c>
-      <c r="V2" s="2">
+      <c r="V2">
         <v>0.433</v>
       </c>
-      <c r="W2" s="2">
+      <c r="W2">
         <v>0.433</v>
       </c>
-      <c r="X2" s="2">
+      <c r="X2">
         <v>2.6</v>
       </c>
-      <c r="Y2" s="2">
+      <c r="Y2">
         <v>5</v>
       </c>
-      <c r="Z2" s="2">
+      <c r="Z2">
         <v>0.526</v>
       </c>
-      <c r="AA2" s="2"/>
-      <c r="AB2" s="2"/>
-      <c r="AC2" s="2">
+      <c r="AC2">
         <v>19.3</v>
       </c>
-      <c r="AD2" s="2">
+      <c r="AD2">
         <v>4.9</v>
       </c>
-      <c r="AE2" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AF2" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AG2" s="2"/>
-      <c r="AH2" s="2">
+      <c r="AE2" t="s">
+        <v>91</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>91</v>
+      </c>
+      <c r="AH2">
         <v>3</v>
       </c>
-      <c r="AI2" s="2">
+      <c r="AI2">
         <v>9.9</v>
       </c>
-      <c r="AJ2" s="2" t="s">
+      <c r="AJ2" t="s">
         <v>92</v>
       </c>
-      <c r="AK2" s="2" t="s">
+      <c r="AK2" t="s">
         <v>102</v>
       </c>
-      <c r="AL2" s="2" t="s">
+      <c r="AL2" t="s">
         <v>102</v>
       </c>
-      <c r="AM2" s="2">
+      <c r="AM2">
         <v>1969</v>
       </c>
-      <c r="AN2" s="2">
+      <c r="AN2">
         <v>3901</v>
       </c>
-      <c r="AO2" s="2">
+      <c r="AO2">
         <v>699</v>
       </c>
-      <c r="AP2" s="2" t="s">
+      <c r="AP2" t="s">
         <v>104</v>
       </c>
-      <c r="AQ2" s="2">
+      <c r="AQ2">
         <v>1937</v>
       </c>
-      <c r="AR2" s="2" t="s">
+      <c r="AR2" t="s">
         <v>88</v>
       </c>
-      <c r="AS2" s="2">
+      <c r="AS2">
         <v>32</v>
       </c>
-      <c r="AT2" s="2">
+      <c r="AT2">
         <v>10</v>
       </c>
-      <c r="AU2" s="2" t="s">
+      <c r="AU2" t="s">
         <v>89</v>
       </c>
-      <c r="AV2" s="2" t="s">
+      <c r="AV2" t="s">
         <v>105</v>
       </c>
-      <c r="AW2" s="2">
+      <c r="AW2">
         <v>81</v>
       </c>
-      <c r="AX2" s="2"/>
-      <c r="AY2" s="2">
+      <c r="AY2">
         <v>45.3</v>
       </c>
-      <c r="AZ2" s="2">
+      <c r="AZ2">
         <v>7.9</v>
       </c>
-      <c r="BA2" s="2">
+      <c r="BA2">
         <v>13.6</v>
       </c>
-      <c r="BB2" s="2">
+      <c r="BB2">
         <v>0.583</v>
       </c>
-      <c r="BC2" s="2"/>
-      <c r="BD2" s="2"/>
-      <c r="BE2" s="2"/>
-      <c r="BF2" s="2">
+      <c r="BF2">
         <v>7.9</v>
       </c>
-      <c r="BG2" s="2">
+      <c r="BG2">
         <v>13.6</v>
       </c>
-      <c r="BH2" s="2">
+      <c r="BH2">
         <v>0.583</v>
       </c>
-      <c r="BI2" s="2">
+      <c r="BI2">
         <v>0.583</v>
       </c>
-      <c r="BJ2" s="2">
+      <c r="BJ2">
         <v>4.7</v>
       </c>
-      <c r="BK2" s="2">
+      <c r="BK2">
         <v>10.6</v>
       </c>
-      <c r="BL2" s="2">
+      <c r="BL2">
         <v>0.446</v>
       </c>
-      <c r="BM2" s="2"/>
-      <c r="BN2" s="2"/>
-      <c r="BO2" s="2">
+      <c r="BO2">
         <v>21.1</v>
       </c>
-      <c r="BP2" s="2">
+      <c r="BP2">
         <v>4.5</v>
       </c>
-      <c r="BQ2" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="BR2" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="BS2" s="2"/>
-      <c r="BT2" s="2">
+      <c r="BQ2" t="s">
+        <v>91</v>
+      </c>
+      <c r="BR2" t="s">
+        <v>91</v>
+      </c>
+      <c r="BT2">
         <v>1.8</v>
       </c>
-      <c r="BU2" s="2">
+      <c r="BU2">
         <v>20.5</v>
       </c>
-      <c r="BV2" s="2" t="s">
+      <c r="BV2" t="s">
         <v>92</v>
       </c>
-      <c r="BW2" s="2" t="s">
+      <c r="BW2" t="s">
         <v>103</v>
       </c>
-      <c r="BX2" s="2" t="s">
+      <c r="BX2" t="s">
         <v>102</v>
       </c>
-      <c r="BY2" s="2">
+      <c r="BY2">
         <v>1969</v>
       </c>
     </row>
     <row r="3" spans="1:77">
-      <c r="A3" s="2">
+      <c r="A3">
         <v>3150</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" t="s">
         <v>78</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3">
         <v>610</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" t="s">
         <v>87</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3">
         <v>1935</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" t="s">
         <v>88</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3">
         <v>33</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3">
         <v>12</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" t="s">
         <v>89</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J3" t="s">
         <v>90</v>
       </c>
-      <c r="K3" s="2">
+      <c r="K3">
         <v>78</v>
       </c>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2">
+      <c r="M3">
         <v>37.9</v>
       </c>
-      <c r="N3" s="2">
+      <c r="N3">
         <v>4.7</v>
       </c>
-      <c r="O3" s="2">
+      <c r="O3">
         <v>11</v>
       </c>
-      <c r="P3" s="2">
+      <c r="P3">
         <v>0.425</v>
       </c>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
-      <c r="T3" s="2">
+      <c r="T3">
         <v>4.7</v>
       </c>
-      <c r="U3" s="2">
+      <c r="U3">
         <v>11</v>
       </c>
-      <c r="V3" s="2">
+      <c r="V3">
         <v>0.425</v>
       </c>
-      <c r="W3" s="2">
+      <c r="W3">
         <v>0.425</v>
       </c>
-      <c r="X3" s="2">
+      <c r="X3">
         <v>3.2</v>
       </c>
-      <c r="Y3" s="2">
+      <c r="Y3">
         <v>5.9</v>
       </c>
-      <c r="Z3" s="2">
+      <c r="Z3">
         <v>0.537</v>
       </c>
-      <c r="AA3" s="2"/>
-      <c r="AB3" s="2"/>
-      <c r="AC3" s="2">
+      <c r="AC3">
         <v>18.6</v>
       </c>
-      <c r="AD3" s="2">
+      <c r="AD3">
         <v>4.6</v>
       </c>
-      <c r="AE3" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AF3" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AG3" s="2"/>
-      <c r="AH3" s="2">
+      <c r="AE3" t="s">
+        <v>91</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>91</v>
+      </c>
+      <c r="AH3">
         <v>3.1</v>
       </c>
-      <c r="AI3" s="2">
+      <c r="AI3">
         <v>12.5</v>
       </c>
-      <c r="AJ3" s="2" t="s">
+      <c r="AJ3" t="s">
         <v>93</v>
       </c>
-      <c r="AK3" s="2" t="s">
+      <c r="AK3" t="s">
         <v>103</v>
       </c>
-      <c r="AL3" s="2" t="s">
+      <c r="AL3" t="s">
         <v>102</v>
       </c>
-      <c r="AM3" s="2">
+      <c r="AM3">
         <v>1968</v>
       </c>
-      <c r="AN3" s="2">
+      <c r="AN3">
         <v>3485</v>
       </c>
-      <c r="AO3" s="2">
+      <c r="AO3">
         <v>699</v>
       </c>
-      <c r="AP3" s="2" t="s">
+      <c r="AP3" t="s">
         <v>104</v>
       </c>
-      <c r="AQ3" s="2">
+      <c r="AQ3">
         <v>1937</v>
       </c>
-      <c r="AR3" s="2" t="s">
+      <c r="AR3" t="s">
         <v>88</v>
       </c>
-      <c r="AS3" s="2">
+      <c r="AS3">
         <v>31</v>
       </c>
-      <c r="AT3" s="2">
+      <c r="AT3">
         <v>9</v>
       </c>
-      <c r="AU3" s="2" t="s">
+      <c r="AU3" t="s">
         <v>89</v>
       </c>
-      <c r="AV3" s="2" t="s">
+      <c r="AV3" t="s">
         <v>106</v>
       </c>
-      <c r="AW3" s="2">
+      <c r="AW3">
         <v>82</v>
       </c>
-      <c r="AX3" s="2"/>
-      <c r="AY3" s="2">
+      <c r="AY3">
         <v>46.8</v>
       </c>
-      <c r="AZ3" s="2">
+      <c r="AZ3">
         <v>10</v>
       </c>
-      <c r="BA3" s="2">
+      <c r="BA3">
         <v>16.8</v>
       </c>
-      <c r="BB3" s="2">
+      <c r="BB3">
         <v>0.595</v>
       </c>
-      <c r="BC3" s="2"/>
-      <c r="BD3" s="2"/>
-      <c r="BE3" s="2"/>
-      <c r="BF3" s="2">
+      <c r="BF3">
         <v>10</v>
       </c>
-      <c r="BG3" s="2">
+      <c r="BG3">
         <v>16.8</v>
       </c>
-      <c r="BH3" s="2">
+      <c r="BH3">
         <v>0.595</v>
       </c>
-      <c r="BI3" s="2">
+      <c r="BI3">
         <v>0.595</v>
       </c>
-      <c r="BJ3" s="2">
+      <c r="BJ3">
         <v>4.3</v>
       </c>
-      <c r="BK3" s="2">
+      <c r="BK3">
         <v>11.4</v>
       </c>
-      <c r="BL3" s="2">
+      <c r="BL3">
         <v>0.38</v>
       </c>
-      <c r="BM3" s="2"/>
-      <c r="BN3" s="2"/>
-      <c r="BO3" s="2">
+      <c r="BO3">
         <v>23.8</v>
       </c>
-      <c r="BP3" s="3">
+      <c r="BP3">
         <v>8.6</v>
       </c>
-      <c r="BQ3" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="BR3" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="BS3" s="2"/>
-      <c r="BT3" s="2">
+      <c r="BQ3" t="s">
+        <v>91</v>
+      </c>
+      <c r="BR3" t="s">
+        <v>91</v>
+      </c>
+      <c r="BT3">
         <v>2</v>
       </c>
-      <c r="BU3" s="2">
+      <c r="BU3">
         <v>24.3</v>
       </c>
-      <c r="BV3" s="2" t="s">
+      <c r="BV3" t="s">
         <v>93</v>
       </c>
-      <c r="BW3" s="2" t="s">
+      <c r="BW3" t="s">
         <v>103</v>
       </c>
-      <c r="BX3" s="2" t="s">
+      <c r="BX3" t="s">
         <v>102</v>
       </c>
-      <c r="BY3" s="2">
+      <c r="BY3">
         <v>1968</v>
       </c>
     </row>
     <row r="4" spans="1:77">
-      <c r="A4" s="2">
+      <c r="A4">
         <v>2995</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" t="s">
         <v>79</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4">
         <v>610</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" t="s">
         <v>87</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4">
         <v>1935</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" t="s">
         <v>88</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4">
         <v>32</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4">
         <v>11</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" t="s">
         <v>89</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="J4" t="s">
         <v>90</v>
       </c>
-      <c r="K4" s="2">
+      <c r="K4">
         <v>81</v>
       </c>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2">
+      <c r="M4">
         <v>40.7</v>
       </c>
-      <c r="N4" s="2">
+      <c r="N4">
         <v>4.9</v>
       </c>
-      <c r="O4" s="2">
+      <c r="O4">
         <v>10.7</v>
       </c>
-      <c r="P4" s="2">
+      <c r="P4">
         <v>0.454</v>
       </c>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
-      <c r="T4" s="2">
+      <c r="T4">
         <v>4.9</v>
       </c>
-      <c r="U4" s="2">
+      <c r="U4">
         <v>10.7</v>
       </c>
-      <c r="V4" s="2">
+      <c r="V4">
         <v>0.454</v>
       </c>
-      <c r="W4" s="2">
+      <c r="W4">
         <v>0.454</v>
       </c>
-      <c r="X4" s="2">
+      <c r="X4">
         <v>3.5</v>
       </c>
-      <c r="Y4" s="2">
+      <c r="Y4">
         <v>5.8</v>
       </c>
-      <c r="Z4" s="2">
+      <c r="Z4">
         <v>0.61</v>
       </c>
-      <c r="AA4" s="2"/>
-      <c r="AB4" s="2"/>
-      <c r="AC4" s="2">
+      <c r="AC4">
         <v>21</v>
       </c>
-      <c r="AD4" s="3">
+      <c r="AD4">
         <v>5.8</v>
       </c>
-      <c r="AE4" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AF4" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AG4" s="2"/>
-      <c r="AH4" s="2">
+      <c r="AE4" t="s">
+        <v>91</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>91</v>
+      </c>
+      <c r="AH4">
         <v>3.2</v>
       </c>
-      <c r="AI4" s="2">
+      <c r="AI4">
         <v>13.3</v>
       </c>
-      <c r="AJ4" s="2" t="s">
+      <c r="AJ4" t="s">
         <v>94</v>
       </c>
-      <c r="AK4" s="2" t="s">
+      <c r="AK4" t="s">
         <v>103</v>
       </c>
-      <c r="AL4" s="2" t="s">
+      <c r="AL4" t="s">
         <v>102</v>
       </c>
-      <c r="AM4" s="2">
+      <c r="AM4">
         <v>1967</v>
       </c>
-      <c r="AN4" s="2">
+      <c r="AN4">
         <v>3118</v>
       </c>
-      <c r="AO4" s="2">
+      <c r="AO4">
         <v>699</v>
       </c>
-      <c r="AP4" s="2" t="s">
+      <c r="AP4" t="s">
         <v>104</v>
       </c>
-      <c r="AQ4" s="2">
+      <c r="AQ4">
         <v>1937</v>
       </c>
-      <c r="AR4" s="2" t="s">
+      <c r="AR4" t="s">
         <v>88</v>
       </c>
-      <c r="AS4" s="2">
+      <c r="AS4">
         <v>30</v>
       </c>
-      <c r="AT4" s="2">
+      <c r="AT4">
         <v>8</v>
       </c>
-      <c r="AU4" s="2" t="s">
+      <c r="AU4" t="s">
         <v>89</v>
       </c>
-      <c r="AV4" s="2" t="s">
+      <c r="AV4" t="s">
         <v>106</v>
       </c>
-      <c r="AW4" s="2">
+      <c r="AW4">
         <v>81</v>
       </c>
-      <c r="AX4" s="2"/>
-      <c r="AY4" s="2">
+      <c r="AY4">
         <v>45.5</v>
       </c>
-      <c r="AZ4" s="2">
+      <c r="AZ4">
         <v>9.699999999999999</v>
       </c>
-      <c r="BA4" s="2">
+      <c r="BA4">
         <v>14.2</v>
       </c>
-      <c r="BB4" s="2">
+      <c r="BB4">
         <v>0.6830000000000001</v>
       </c>
-      <c r="BC4" s="2"/>
-      <c r="BD4" s="2"/>
-      <c r="BE4" s="2"/>
-      <c r="BF4" s="2">
+      <c r="BF4">
         <v>9.699999999999999</v>
       </c>
-      <c r="BG4" s="2">
+      <c r="BG4">
         <v>14.2</v>
       </c>
-      <c r="BH4" s="2">
+      <c r="BH4">
         <v>0.6830000000000001</v>
       </c>
-      <c r="BI4" s="2">
+      <c r="BI4">
         <v>0.6830000000000001</v>
       </c>
-      <c r="BJ4" s="2">
+      <c r="BJ4">
         <v>4.8</v>
       </c>
-      <c r="BK4" s="2">
+      <c r="BK4">
         <v>10.8</v>
       </c>
-      <c r="BL4" s="2">
+      <c r="BL4">
         <v>0.441</v>
       </c>
-      <c r="BM4" s="2"/>
-      <c r="BN4" s="2"/>
-      <c r="BO4" s="2">
+      <c r="BO4">
         <v>24.2</v>
       </c>
-      <c r="BP4" s="2">
+      <c r="BP4">
         <v>7.8</v>
       </c>
-      <c r="BQ4" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="BR4" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="BS4" s="2"/>
-      <c r="BT4" s="2">
+      <c r="BQ4" t="s">
+        <v>91</v>
+      </c>
+      <c r="BR4" t="s">
+        <v>91</v>
+      </c>
+      <c r="BT4">
         <v>1.8</v>
       </c>
-      <c r="BU4" s="2">
+      <c r="BU4">
         <v>24.1</v>
       </c>
-      <c r="BV4" s="2" t="s">
+      <c r="BV4" t="s">
         <v>94</v>
       </c>
-      <c r="BW4" s="2" t="s">
+      <c r="BW4" t="s">
         <v>103</v>
       </c>
-      <c r="BX4" s="2" t="s">
+      <c r="BX4" t="s">
         <v>102</v>
       </c>
-      <c r="BY4" s="2">
+      <c r="BY4">
         <v>1967</v>
       </c>
     </row>
     <row r="5" spans="1:77">
-      <c r="A5" s="2">
+      <c r="A5">
         <v>2865</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" t="s">
         <v>80</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5">
         <v>610</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" t="s">
         <v>87</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5">
         <v>1935</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" t="s">
         <v>88</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5">
         <v>31</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5">
         <v>10</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="I5" t="s">
         <v>89</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="J5" t="s">
         <v>90</v>
       </c>
-      <c r="K5" s="2">
+      <c r="K5">
         <v>78</v>
       </c>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2">
+      <c r="M5">
         <v>43.4</v>
       </c>
-      <c r="N5" s="2">
+      <c r="N5">
         <v>5</v>
       </c>
-      <c r="O5" s="2">
+      <c r="O5">
         <v>12.1</v>
       </c>
-      <c r="P5" s="2">
+      <c r="P5">
         <v>0.415</v>
       </c>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="2"/>
-      <c r="S5" s="2"/>
-      <c r="T5" s="2">
+      <c r="T5">
         <v>5</v>
       </c>
-      <c r="U5" s="2">
+      <c r="U5">
         <v>12.1</v>
       </c>
-      <c r="V5" s="2">
+      <c r="V5">
         <v>0.415</v>
       </c>
-      <c r="W5" s="2">
+      <c r="W5">
         <v>0.415</v>
       </c>
-      <c r="X5" s="2">
+      <c r="X5">
         <v>2.9</v>
       </c>
-      <c r="Y5" s="2">
+      <c r="Y5">
         <v>5.2</v>
       </c>
-      <c r="Z5" s="2">
+      <c r="Z5">
         <v>0.551</v>
       </c>
-      <c r="AA5" s="2"/>
-      <c r="AB5" s="2"/>
-      <c r="AC5" s="2">
+      <c r="AC5">
         <v>22.8</v>
       </c>
-      <c r="AD5" s="2">
+      <c r="AD5">
         <v>4.8</v>
       </c>
-      <c r="AE5" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AF5" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AG5" s="2"/>
-      <c r="AH5" s="2">
+      <c r="AE5" t="s">
+        <v>91</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>91</v>
+      </c>
+      <c r="AH5">
         <v>2.8</v>
       </c>
-      <c r="AI5" s="2">
+      <c r="AI5">
         <v>12.9</v>
       </c>
-      <c r="AJ5" s="2" t="s">
+      <c r="AJ5" t="s">
         <v>95</v>
       </c>
-      <c r="AK5" s="2" t="s">
+      <c r="AK5" t="s">
         <v>103</v>
       </c>
-      <c r="AL5" s="2" t="s">
+      <c r="AL5" t="s">
         <v>102</v>
       </c>
-      <c r="AM5" s="2">
+      <c r="AM5">
         <v>1966</v>
       </c>
-      <c r="AN5" s="2">
+      <c r="AN5">
         <v>2984</v>
       </c>
-      <c r="AO5" s="2">
+      <c r="AO5">
         <v>699</v>
       </c>
-      <c r="AP5" s="2" t="s">
+      <c r="AP5" t="s">
         <v>104</v>
       </c>
-      <c r="AQ5" s="2">
+      <c r="AQ5">
         <v>1937</v>
       </c>
-      <c r="AR5" s="2" t="s">
+      <c r="AR5" t="s">
         <v>88</v>
       </c>
-      <c r="AS5" s="2">
+      <c r="AS5">
         <v>29</v>
       </c>
-      <c r="AT5" s="2">
+      <c r="AT5">
         <v>7</v>
       </c>
-      <c r="AU5" s="2" t="s">
+      <c r="AU5" t="s">
         <v>89</v>
       </c>
-      <c r="AV5" s="2" t="s">
+      <c r="AV5" t="s">
         <v>106</v>
       </c>
-      <c r="AW5" s="2">
+      <c r="AW5">
         <v>79</v>
       </c>
-      <c r="AX5" s="2"/>
-      <c r="AY5" s="2">
+      <c r="AY5">
         <v>47.3</v>
       </c>
-      <c r="AZ5" s="2">
+      <c r="AZ5">
         <v>13.6</v>
       </c>
-      <c r="BA5" s="2">
+      <c r="BA5">
         <v>25.2</v>
       </c>
-      <c r="BB5" s="2">
+      <c r="BB5">
         <v>0.54</v>
       </c>
-      <c r="BC5" s="2"/>
-      <c r="BD5" s="2"/>
-      <c r="BE5" s="2"/>
-      <c r="BF5" s="2">
+      <c r="BF5">
         <v>13.6</v>
       </c>
-      <c r="BG5" s="2">
+      <c r="BG5">
         <v>25.2</v>
       </c>
-      <c r="BH5" s="2">
+      <c r="BH5">
         <v>0.54</v>
       </c>
-      <c r="BI5" s="2">
+      <c r="BI5">
         <v>0.54</v>
       </c>
-      <c r="BJ5" s="2">
+      <c r="BJ5">
         <v>6.3</v>
       </c>
-      <c r="BK5" s="2">
+      <c r="BK5">
         <v>12.4</v>
       </c>
-      <c r="BL5" s="2">
+      <c r="BL5">
         <v>0.513</v>
       </c>
-      <c r="BM5" s="2"/>
-      <c r="BN5" s="2"/>
-      <c r="BO5" s="2">
+      <c r="BO5">
         <v>24.6</v>
       </c>
-      <c r="BP5" s="2">
+      <c r="BP5">
         <v>5.2</v>
       </c>
-      <c r="BQ5" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="BR5" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="BS5" s="2"/>
-      <c r="BT5" s="2">
+      <c r="BQ5" t="s">
+        <v>91</v>
+      </c>
+      <c r="BR5" t="s">
+        <v>91</v>
+      </c>
+      <c r="BT5">
         <v>2.2</v>
       </c>
-      <c r="BU5" s="2">
+      <c r="BU5">
         <v>33.5</v>
       </c>
-      <c r="BV5" s="2" t="s">
+      <c r="BV5" t="s">
         <v>95</v>
       </c>
-      <c r="BW5" s="2" t="s">
+      <c r="BW5" t="s">
         <v>103</v>
       </c>
-      <c r="BX5" s="2" t="s">
+      <c r="BX5" t="s">
         <v>102</v>
       </c>
-      <c r="BY5" s="2">
+      <c r="BY5">
         <v>1966</v>
       </c>
     </row>
     <row r="6" spans="1:77">
-      <c r="A6" s="2">
+      <c r="A6">
         <v>2735</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" t="s">
         <v>81</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6">
         <v>610</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" t="s">
         <v>87</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6">
         <v>1935</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" t="s">
         <v>88</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6">
         <v>30</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6">
         <v>9</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="I6" t="s">
         <v>89</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="J6" t="s">
         <v>90</v>
       </c>
-      <c r="K6" s="2">
+      <c r="K6">
         <v>78</v>
       </c>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2">
+      <c r="M6">
         <v>44.4</v>
       </c>
-      <c r="N6" s="2">
+      <c r="N6">
         <v>5.5</v>
       </c>
-      <c r="O6" s="2">
+      <c r="O6">
         <v>12.6</v>
       </c>
-      <c r="P6" s="2">
+      <c r="P6">
         <v>0.438</v>
       </c>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="2"/>
-      <c r="S6" s="2"/>
-      <c r="T6" s="2">
+      <c r="T6">
         <v>5.5</v>
       </c>
-      <c r="U6" s="2">
+      <c r="U6">
         <v>12.6</v>
       </c>
-      <c r="V6" s="2">
+      <c r="V6">
         <v>0.438</v>
       </c>
-      <c r="W6" s="2">
+      <c r="W6">
         <v>0.438</v>
       </c>
-      <c r="X6" s="2">
+      <c r="X6">
         <v>3.1</v>
       </c>
-      <c r="Y6" s="2">
+      <c r="Y6">
         <v>5.5</v>
       </c>
-      <c r="Z6" s="2">
+      <c r="Z6">
         <v>0.573</v>
       </c>
-      <c r="AA6" s="2"/>
-      <c r="AB6" s="2"/>
-      <c r="AC6" s="2">
+      <c r="AC6">
         <v>24.1</v>
       </c>
-      <c r="AD6" s="2">
+      <c r="AD6">
         <v>5.3</v>
       </c>
-      <c r="AE6" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AF6" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AG6" s="2"/>
-      <c r="AH6" s="2">
+      <c r="AE6" t="s">
+        <v>91</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>91</v>
+      </c>
+      <c r="AH6">
         <v>2.6</v>
       </c>
-      <c r="AI6" s="2">
+      <c r="AI6">
         <v>14.1</v>
       </c>
-      <c r="AJ6" s="2" t="s">
+      <c r="AJ6" t="s">
         <v>96</v>
       </c>
-      <c r="AK6" s="2" t="s">
+      <c r="AK6" t="s">
         <v>103</v>
       </c>
-      <c r="AL6" s="2" t="s">
+      <c r="AL6" t="s">
         <v>102</v>
       </c>
-      <c r="AM6" s="2">
+      <c r="AM6">
         <v>1965</v>
       </c>
-      <c r="AN6" s="2">
+      <c r="AN6">
         <v>2848</v>
       </c>
-      <c r="AO6" s="2">
+      <c r="AO6">
         <v>699</v>
       </c>
-      <c r="AP6" s="2" t="s">
+      <c r="AP6" t="s">
         <v>104</v>
       </c>
-      <c r="AQ6" s="2">
+      <c r="AQ6">
         <v>1937</v>
       </c>
-      <c r="AR6" s="2" t="s">
+      <c r="AR6" t="s">
         <v>88</v>
       </c>
-      <c r="AS6" s="2">
+      <c r="AS6">
         <v>28</v>
       </c>
-      <c r="AT6" s="2">
+      <c r="AT6">
         <v>6</v>
       </c>
-      <c r="AU6" s="2" t="s">
+      <c r="AU6" t="s">
         <v>89</v>
       </c>
-      <c r="AV6" s="2" t="s">
+      <c r="AV6" t="s">
         <v>107</v>
       </c>
-      <c r="AW6" s="2">
+      <c r="AW6">
         <v>73</v>
       </c>
-      <c r="AX6" s="2"/>
-      <c r="AY6" s="2">
+      <c r="AY6">
         <v>45.2</v>
       </c>
-      <c r="AZ6" s="2">
+      <c r="AZ6">
         <v>14.6</v>
       </c>
-      <c r="BA6" s="2">
+      <c r="BA6">
         <v>28.5</v>
       </c>
-      <c r="BB6" s="2">
+      <c r="BB6">
         <v>0.51</v>
       </c>
-      <c r="BC6" s="2"/>
-      <c r="BD6" s="2"/>
-      <c r="BE6" s="2"/>
-      <c r="BF6" s="2">
+      <c r="BF6">
         <v>14.6</v>
       </c>
-      <c r="BG6" s="2">
+      <c r="BG6">
         <v>28.5</v>
       </c>
-      <c r="BH6" s="2">
+      <c r="BH6">
         <v>0.51</v>
       </c>
-      <c r="BI6" s="2">
+      <c r="BI6">
         <v>0.51</v>
       </c>
-      <c r="BJ6" s="2">
+      <c r="BJ6">
         <v>5.6</v>
       </c>
-      <c r="BK6" s="2">
+      <c r="BK6">
         <v>12.1</v>
       </c>
-      <c r="BL6" s="2">
+      <c r="BL6">
         <v>0.464</v>
       </c>
-      <c r="BM6" s="2"/>
-      <c r="BN6" s="2"/>
-      <c r="BO6" s="2">
+      <c r="BO6">
         <v>22.9</v>
       </c>
-      <c r="BP6" s="2">
+      <c r="BP6">
         <v>3.4</v>
       </c>
-      <c r="BQ6" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="BR6" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="BS6" s="2"/>
-      <c r="BT6" s="2">
+      <c r="BQ6" t="s">
+        <v>91</v>
+      </c>
+      <c r="BR6" t="s">
+        <v>91</v>
+      </c>
+      <c r="BT6">
         <v>2</v>
       </c>
-      <c r="BU6" s="2">
+      <c r="BU6">
         <v>34.7</v>
       </c>
-      <c r="BV6" s="2" t="s">
+      <c r="BV6" t="s">
         <v>96</v>
       </c>
-      <c r="BW6" s="2" t="s">
+      <c r="BW6" t="s">
         <v>103</v>
       </c>
-      <c r="BX6" s="2" t="s">
+      <c r="BX6" t="s">
         <v>102</v>
       </c>
-      <c r="BY6" s="2">
+      <c r="BY6">
         <v>1965</v>
       </c>
     </row>
     <row r="7" spans="1:77">
-      <c r="A7" s="2">
+      <c r="A7">
         <v>2735</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" t="s">
         <v>81</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7">
         <v>610</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" t="s">
         <v>87</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7">
         <v>1935</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" t="s">
         <v>88</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7">
         <v>30</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7">
         <v>9</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="I7" t="s">
         <v>89</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="J7" t="s">
         <v>90</v>
       </c>
-      <c r="K7" s="2">
+      <c r="K7">
         <v>78</v>
       </c>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2">
+      <c r="M7">
         <v>44.4</v>
       </c>
-      <c r="N7" s="2">
+      <c r="N7">
         <v>5.5</v>
       </c>
-      <c r="O7" s="2">
+      <c r="O7">
         <v>12.6</v>
       </c>
-      <c r="P7" s="2">
+      <c r="P7">
         <v>0.438</v>
       </c>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
-      <c r="S7" s="2"/>
-      <c r="T7" s="2">
+      <c r="T7">
         <v>5.5</v>
       </c>
-      <c r="U7" s="2">
+      <c r="U7">
         <v>12.6</v>
       </c>
-      <c r="V7" s="2">
+      <c r="V7">
         <v>0.438</v>
       </c>
-      <c r="W7" s="2">
+      <c r="W7">
         <v>0.438</v>
       </c>
-      <c r="X7" s="2">
+      <c r="X7">
         <v>3.1</v>
       </c>
-      <c r="Y7" s="2">
+      <c r="Y7">
         <v>5.5</v>
       </c>
-      <c r="Z7" s="2">
+      <c r="Z7">
         <v>0.573</v>
       </c>
-      <c r="AA7" s="2"/>
-      <c r="AB7" s="2"/>
-      <c r="AC7" s="2">
+      <c r="AC7">
         <v>24.1</v>
       </c>
-      <c r="AD7" s="2">
+      <c r="AD7">
         <v>5.3</v>
       </c>
-      <c r="AE7" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AF7" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AG7" s="2"/>
-      <c r="AH7" s="2">
+      <c r="AE7" t="s">
+        <v>91</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>91</v>
+      </c>
+      <c r="AH7">
         <v>2.6</v>
       </c>
-      <c r="AI7" s="2">
+      <c r="AI7">
         <v>14.1</v>
       </c>
-      <c r="AJ7" s="2" t="s">
+      <c r="AJ7" t="s">
         <v>96</v>
       </c>
-      <c r="AK7" s="2" t="s">
+      <c r="AK7" t="s">
         <v>103</v>
       </c>
-      <c r="AL7" s="2" t="s">
+      <c r="AL7" t="s">
         <v>102</v>
       </c>
-      <c r="AM7" s="2">
+      <c r="AM7">
         <v>1965</v>
       </c>
-      <c r="AN7" s="2">
+      <c r="AN7">
         <v>2849</v>
       </c>
-      <c r="AO7" s="2">
+      <c r="AO7">
         <v>699</v>
       </c>
-      <c r="AP7" s="2" t="s">
+      <c r="AP7" t="s">
         <v>104</v>
       </c>
-      <c r="AQ7" s="2">
+      <c r="AQ7">
         <v>1937</v>
       </c>
-      <c r="AR7" s="2" t="s">
+      <c r="AR7" t="s">
         <v>88</v>
       </c>
-      <c r="AS7" s="2">
+      <c r="AS7">
         <v>28</v>
       </c>
-      <c r="AT7" s="2">
+      <c r="AT7">
         <v>6</v>
       </c>
-      <c r="AU7" s="2" t="s">
+      <c r="AU7" t="s">
         <v>89</v>
       </c>
-      <c r="AV7" s="2" t="s">
+      <c r="AV7" t="s">
         <v>108</v>
       </c>
-      <c r="AW7" s="2">
+      <c r="AW7">
         <v>38</v>
       </c>
-      <c r="AX7" s="2"/>
-      <c r="AY7" s="2">
+      <c r="AY7">
         <v>45.9</v>
       </c>
-      <c r="AZ7" s="2">
+      <c r="AZ7">
         <v>16.7</v>
       </c>
-      <c r="BA7" s="2">
+      <c r="BA7">
         <v>33.6</v>
       </c>
-      <c r="BB7" s="2">
+      <c r="BB7">
         <v>0.499</v>
       </c>
-      <c r="BC7" s="2"/>
-      <c r="BD7" s="2"/>
-      <c r="BE7" s="2"/>
-      <c r="BF7" s="2">
+      <c r="BF7">
         <v>16.7</v>
       </c>
-      <c r="BG7" s="2">
+      <c r="BG7">
         <v>33.6</v>
       </c>
-      <c r="BH7" s="2">
+      <c r="BH7">
         <v>0.499</v>
       </c>
-      <c r="BI7" s="2">
+      <c r="BI7">
         <v>0.499</v>
       </c>
-      <c r="BJ7" s="2">
+      <c r="BJ7">
         <v>5.5</v>
       </c>
-      <c r="BK7" s="2">
+      <c r="BK7">
         <v>13.2</v>
       </c>
-      <c r="BL7" s="2">
+      <c r="BL7">
         <v>0.416</v>
       </c>
-      <c r="BM7" s="2"/>
-      <c r="BN7" s="2"/>
-      <c r="BO7" s="2">
+      <c r="BO7">
         <v>23.5</v>
       </c>
-      <c r="BP7" s="2">
+      <c r="BP7">
         <v>3.1</v>
       </c>
-      <c r="BQ7" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="BR7" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="BS7" s="2"/>
-      <c r="BT7" s="2">
+      <c r="BQ7" t="s">
+        <v>91</v>
+      </c>
+      <c r="BR7" t="s">
+        <v>91</v>
+      </c>
+      <c r="BT7">
         <v>2</v>
       </c>
-      <c r="BU7" s="2">
+      <c r="BU7">
         <v>38.9</v>
       </c>
-      <c r="BV7" s="2" t="s">
+      <c r="BV7" t="s">
         <v>96</v>
       </c>
-      <c r="BW7" s="2" t="s">
+      <c r="BW7" t="s">
         <v>103</v>
       </c>
-      <c r="BX7" s="2" t="s">
+      <c r="BX7" t="s">
         <v>102</v>
       </c>
-      <c r="BY7" s="2">
+      <c r="BY7">
         <v>1965</v>
       </c>
     </row>
     <row r="8" spans="1:77">
-      <c r="A8" s="2">
+      <c r="A8">
         <v>2735</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" t="s">
         <v>81</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8">
         <v>610</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" t="s">
         <v>87</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8">
         <v>1935</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" t="s">
         <v>88</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8">
         <v>30</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8">
         <v>9</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="I8" t="s">
         <v>89</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="J8" t="s">
         <v>90</v>
       </c>
-      <c r="K8" s="2">
+      <c r="K8">
         <v>78</v>
       </c>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2">
+      <c r="M8">
         <v>44.4</v>
       </c>
-      <c r="N8" s="2">
+      <c r="N8">
         <v>5.5</v>
       </c>
-      <c r="O8" s="2">
+      <c r="O8">
         <v>12.6</v>
       </c>
-      <c r="P8" s="2">
+      <c r="P8">
         <v>0.438</v>
       </c>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="2"/>
-      <c r="S8" s="2"/>
-      <c r="T8" s="2">
+      <c r="T8">
         <v>5.5</v>
       </c>
-      <c r="U8" s="2">
+      <c r="U8">
         <v>12.6</v>
       </c>
-      <c r="V8" s="2">
+      <c r="V8">
         <v>0.438</v>
       </c>
-      <c r="W8" s="2">
+      <c r="W8">
         <v>0.438</v>
       </c>
-      <c r="X8" s="2">
+      <c r="X8">
         <v>3.1</v>
       </c>
-      <c r="Y8" s="2">
+      <c r="Y8">
         <v>5.5</v>
       </c>
-      <c r="Z8" s="2">
+      <c r="Z8">
         <v>0.573</v>
       </c>
-      <c r="AA8" s="2"/>
-      <c r="AB8" s="2"/>
-      <c r="AC8" s="2">
+      <c r="AC8">
         <v>24.1</v>
       </c>
-      <c r="AD8" s="2">
+      <c r="AD8">
         <v>5.3</v>
       </c>
-      <c r="AE8" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AF8" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AG8" s="2"/>
-      <c r="AH8" s="2">
+      <c r="AE8" t="s">
+        <v>91</v>
+      </c>
+      <c r="AF8" t="s">
+        <v>91</v>
+      </c>
+      <c r="AH8">
         <v>2.6</v>
       </c>
-      <c r="AI8" s="2">
+      <c r="AI8">
         <v>14.1</v>
       </c>
-      <c r="AJ8" s="2" t="s">
+      <c r="AJ8" t="s">
         <v>96</v>
       </c>
-      <c r="AK8" s="2" t="s">
+      <c r="AK8" t="s">
         <v>103</v>
       </c>
-      <c r="AL8" s="2" t="s">
+      <c r="AL8" t="s">
         <v>102</v>
       </c>
-      <c r="AM8" s="2">
+      <c r="AM8">
         <v>1965</v>
       </c>
-      <c r="AN8" s="2">
+      <c r="AN8">
         <v>2850</v>
       </c>
-      <c r="AO8" s="2">
+      <c r="AO8">
         <v>699</v>
       </c>
-      <c r="AP8" s="2" t="s">
+      <c r="AP8" t="s">
         <v>104</v>
       </c>
-      <c r="AQ8" s="2">
+      <c r="AQ8">
         <v>1937</v>
       </c>
-      <c r="AR8" s="2" t="s">
+      <c r="AR8" t="s">
         <v>88</v>
       </c>
-      <c r="AS8" s="2">
+      <c r="AS8">
         <v>28</v>
       </c>
-      <c r="AT8" s="2">
+      <c r="AT8">
         <v>6</v>
       </c>
-      <c r="AU8" s="2" t="s">
+      <c r="AU8" t="s">
         <v>89</v>
       </c>
-      <c r="AV8" s="2" t="s">
+      <c r="AV8" t="s">
         <v>106</v>
       </c>
-      <c r="AW8" s="2">
+      <c r="AW8">
         <v>35</v>
       </c>
-      <c r="AX8" s="2"/>
-      <c r="AY8" s="2">
+      <c r="AY8">
         <v>44.5</v>
       </c>
-      <c r="AZ8" s="2">
+      <c r="AZ8">
         <v>12.2</v>
       </c>
-      <c r="BA8" s="2">
+      <c r="BA8">
         <v>23.1</v>
       </c>
-      <c r="BB8" s="2">
+      <c r="BB8">
         <v>0.528</v>
       </c>
-      <c r="BC8" s="2"/>
-      <c r="BD8" s="2"/>
-      <c r="BE8" s="2"/>
-      <c r="BF8" s="2">
+      <c r="BF8">
         <v>12.2</v>
       </c>
-      <c r="BG8" s="2">
+      <c r="BG8">
         <v>23.1</v>
       </c>
-      <c r="BH8" s="2">
+      <c r="BH8">
         <v>0.528</v>
       </c>
-      <c r="BI8" s="2">
+      <c r="BI8">
         <v>0.528</v>
       </c>
-      <c r="BJ8" s="2">
+      <c r="BJ8">
         <v>5.7</v>
       </c>
-      <c r="BK8" s="2">
+      <c r="BK8">
         <v>10.9</v>
       </c>
-      <c r="BL8" s="2">
+      <c r="BL8">
         <v>0.526</v>
       </c>
-      <c r="BM8" s="2"/>
-      <c r="BN8" s="2"/>
-      <c r="BO8" s="2">
+      <c r="BO8">
         <v>22.3</v>
       </c>
-      <c r="BP8" s="2">
+      <c r="BP8">
         <v>3.8</v>
       </c>
-      <c r="BQ8" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="BR8" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="BS8" s="2"/>
-      <c r="BT8" s="2">
+      <c r="BQ8" t="s">
+        <v>91</v>
+      </c>
+      <c r="BR8" t="s">
+        <v>91</v>
+      </c>
+      <c r="BT8">
         <v>2</v>
       </c>
-      <c r="BU8" s="2">
+      <c r="BU8">
         <v>30.1</v>
       </c>
-      <c r="BV8" s="2" t="s">
+      <c r="BV8" t="s">
         <v>96</v>
       </c>
-      <c r="BW8" s="2" t="s">
+      <c r="BW8" t="s">
         <v>103</v>
       </c>
-      <c r="BX8" s="2" t="s">
+      <c r="BX8" t="s">
         <v>102</v>
       </c>
-      <c r="BY8" s="2">
+      <c r="BY8">
         <v>1965</v>
       </c>
     </row>
     <row r="9" spans="1:77">
-      <c r="A9" s="2">
+      <c r="A9">
         <v>2600</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" t="s">
         <v>82</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9">
         <v>610</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" t="s">
         <v>87</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9">
         <v>1935</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" t="s">
         <v>88</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9">
         <v>29</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9">
         <v>8</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="I9" t="s">
         <v>89</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="J9" t="s">
         <v>90</v>
       </c>
-      <c r="K9" s="2">
+      <c r="K9">
         <v>78</v>
       </c>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2">
+      <c r="M9">
         <v>44.6</v>
       </c>
-      <c r="N9" s="2">
+      <c r="N9">
         <v>6</v>
       </c>
-      <c r="O9" s="2">
+      <c r="O9">
         <v>13.8</v>
       </c>
-      <c r="P9" s="2">
+      <c r="P9">
         <v>0.433</v>
       </c>
-      <c r="Q9" s="2"/>
-      <c r="R9" s="2"/>
-      <c r="S9" s="2"/>
-      <c r="T9" s="2">
+      <c r="T9">
         <v>6</v>
       </c>
-      <c r="U9" s="2">
+      <c r="U9">
         <v>13.8</v>
       </c>
-      <c r="V9" s="2">
+      <c r="V9">
         <v>0.433</v>
       </c>
-      <c r="W9" s="2">
+      <c r="W9">
         <v>0.433</v>
       </c>
-      <c r="X9" s="2">
+      <c r="X9">
         <v>3</v>
       </c>
-      <c r="Y9" s="2">
+      <c r="Y9">
         <v>5.5</v>
       </c>
-      <c r="Z9" s="2">
+      <c r="Z9">
         <v>0.55</v>
       </c>
-      <c r="AA9" s="2"/>
-      <c r="AB9" s="2"/>
-      <c r="AC9" s="3">
+      <c r="AC9">
         <v>24.7</v>
       </c>
-      <c r="AD9" s="2">
+      <c r="AD9">
         <v>4.7</v>
       </c>
-      <c r="AE9" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AF9" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AG9" s="2"/>
-      <c r="AH9" s="2">
+      <c r="AE9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AF9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AH9">
         <v>2.4</v>
       </c>
-      <c r="AI9" s="2">
+      <c r="AI9">
         <v>15</v>
       </c>
-      <c r="AJ9" s="2" t="s">
+      <c r="AJ9" t="s">
         <v>97</v>
       </c>
-      <c r="AK9" s="2" t="s">
+      <c r="AK9" t="s">
         <v>103</v>
       </c>
-      <c r="AL9" s="2" t="s">
+      <c r="AL9" t="s">
         <v>102</v>
       </c>
-      <c r="AM9" s="2">
+      <c r="AM9">
         <v>1964</v>
       </c>
-      <c r="AN9" s="2">
+      <c r="AN9">
         <v>2718</v>
       </c>
-      <c r="AO9" s="2">
+      <c r="AO9">
         <v>699</v>
       </c>
-      <c r="AP9" s="2" t="s">
+      <c r="AP9" t="s">
         <v>104</v>
       </c>
-      <c r="AQ9" s="2">
+      <c r="AQ9">
         <v>1937</v>
       </c>
-      <c r="AR9" s="2" t="s">
+      <c r="AR9" t="s">
         <v>88</v>
       </c>
-      <c r="AS9" s="2">
+      <c r="AS9">
         <v>27</v>
       </c>
-      <c r="AT9" s="2">
+      <c r="AT9">
         <v>5</v>
       </c>
-      <c r="AU9" s="2" t="s">
+      <c r="AU9" t="s">
         <v>89</v>
       </c>
-      <c r="AV9" s="2" t="s">
+      <c r="AV9" t="s">
         <v>108</v>
       </c>
-      <c r="AW9" s="2">
+      <c r="AW9">
         <v>80</v>
       </c>
-      <c r="AX9" s="2"/>
-      <c r="AY9" s="2">
+      <c r="AY9">
         <v>46.1</v>
       </c>
-      <c r="AZ9" s="2">
+      <c r="AZ9">
         <v>15.1</v>
       </c>
-      <c r="BA9" s="2">
+      <c r="BA9">
         <v>28.7</v>
       </c>
-      <c r="BB9" s="2">
+      <c r="BB9">
         <v>0.524</v>
       </c>
-      <c r="BC9" s="2"/>
-      <c r="BD9" s="2"/>
-      <c r="BE9" s="2"/>
-      <c r="BF9" s="2">
+      <c r="BF9">
         <v>15.1</v>
       </c>
-      <c r="BG9" s="2">
+      <c r="BG9">
         <v>28.7</v>
       </c>
-      <c r="BH9" s="2">
+      <c r="BH9">
         <v>0.524</v>
       </c>
-      <c r="BI9" s="2">
+      <c r="BI9">
         <v>0.524</v>
       </c>
-      <c r="BJ9" s="2">
+      <c r="BJ9">
         <v>6.8</v>
       </c>
-      <c r="BK9" s="2">
+      <c r="BK9">
         <v>12.7</v>
       </c>
-      <c r="BL9" s="2">
+      <c r="BL9">
         <v>0.531</v>
       </c>
-      <c r="BM9" s="2"/>
-      <c r="BN9" s="2"/>
-      <c r="BO9" s="2">
+      <c r="BO9">
         <v>22.3</v>
       </c>
-      <c r="BP9" s="2">
+      <c r="BP9">
         <v>5</v>
       </c>
-      <c r="BQ9" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="BR9" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="BS9" s="2"/>
-      <c r="BT9" s="2">
+      <c r="BQ9" t="s">
+        <v>91</v>
+      </c>
+      <c r="BR9" t="s">
+        <v>91</v>
+      </c>
+      <c r="BT9">
         <v>2.3</v>
       </c>
-      <c r="BU9" s="2">
+      <c r="BU9">
         <v>36.9</v>
       </c>
-      <c r="BV9" s="2" t="s">
+      <c r="BV9" t="s">
         <v>97</v>
       </c>
-      <c r="BW9" s="2" t="s">
+      <c r="BW9" t="s">
         <v>103</v>
       </c>
-      <c r="BX9" s="2" t="s">
+      <c r="BX9" t="s">
         <v>102</v>
       </c>
-      <c r="BY9" s="2">
+      <c r="BY9">
         <v>1964</v>
       </c>
     </row>
     <row r="10" spans="1:77">
-      <c r="A10" s="2">
+      <c r="A10">
         <v>2467</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" t="s">
         <v>83</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10">
         <v>610</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" t="s">
         <v>87</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10">
         <v>1935</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" t="s">
         <v>88</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10">
         <v>28</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H10">
         <v>7</v>
       </c>
-      <c r="I10" s="2" t="s">
+      <c r="I10" t="s">
         <v>89</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="J10" t="s">
         <v>90</v>
       </c>
-      <c r="K10" s="2">
+      <c r="K10">
         <v>78</v>
       </c>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2">
+      <c r="M10">
         <v>44.9</v>
       </c>
-      <c r="N10" s="2">
+      <c r="N10">
         <v>6.6</v>
       </c>
-      <c r="O10" s="2">
+      <c r="O10">
         <v>15.2</v>
       </c>
-      <c r="P10" s="2">
+      <c r="P10">
         <v>0.432</v>
       </c>
-      <c r="Q10" s="2"/>
-      <c r="R10" s="2"/>
-      <c r="S10" s="2"/>
-      <c r="T10" s="2">
+      <c r="T10">
         <v>6.6</v>
       </c>
-      <c r="U10" s="2">
+      <c r="U10">
         <v>15.2</v>
       </c>
-      <c r="V10" s="2">
+      <c r="V10">
         <v>0.432</v>
       </c>
-      <c r="W10" s="2">
+      <c r="W10">
         <v>0.432</v>
       </c>
-      <c r="X10" s="2">
+      <c r="X10">
         <v>3.7</v>
       </c>
-      <c r="Y10" s="2">
+      <c r="Y10">
         <v>6.6</v>
       </c>
-      <c r="Z10" s="2">
+      <c r="Z10">
         <v>0.555</v>
       </c>
-      <c r="AA10" s="2"/>
-      <c r="AB10" s="2"/>
-      <c r="AC10" s="2">
+      <c r="AC10">
         <v>23.6</v>
       </c>
-      <c r="AD10" s="2">
+      <c r="AD10">
         <v>4.5</v>
       </c>
-      <c r="AE10" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AF10" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AG10" s="2"/>
-      <c r="AH10" s="2">
+      <c r="AE10" t="s">
+        <v>91</v>
+      </c>
+      <c r="AF10" t="s">
+        <v>91</v>
+      </c>
+      <c r="AH10">
         <v>2.4</v>
       </c>
-      <c r="AI10" s="2">
+      <c r="AI10">
         <v>16.8</v>
       </c>
-      <c r="AJ10" s="2" t="s">
+      <c r="AJ10" t="s">
         <v>98</v>
       </c>
-      <c r="AK10" s="2" t="s">
+      <c r="AK10" t="s">
         <v>103</v>
       </c>
-      <c r="AL10" s="2" t="s">
+      <c r="AL10" t="s">
         <v>102</v>
       </c>
-      <c r="AM10" s="2">
+      <c r="AM10">
         <v>1963</v>
       </c>
-      <c r="AN10" s="2">
+      <c r="AN10">
         <v>2580</v>
       </c>
-      <c r="AO10" s="2">
+      <c r="AO10">
         <v>699</v>
       </c>
-      <c r="AP10" s="2" t="s">
+      <c r="AP10" t="s">
         <v>104</v>
       </c>
-      <c r="AQ10" s="2">
+      <c r="AQ10">
         <v>1937</v>
       </c>
-      <c r="AR10" s="2" t="s">
+      <c r="AR10" t="s">
         <v>88</v>
       </c>
-      <c r="AS10" s="2">
+      <c r="AS10">
         <v>26</v>
       </c>
-      <c r="AT10" s="2">
+      <c r="AT10">
         <v>4</v>
       </c>
-      <c r="AU10" s="2" t="s">
+      <c r="AU10" t="s">
         <v>89</v>
       </c>
-      <c r="AV10" s="2" t="s">
+      <c r="AV10" t="s">
         <v>108</v>
       </c>
-      <c r="AW10" s="2">
+      <c r="AW10">
         <v>80</v>
       </c>
-      <c r="AX10" s="2"/>
-      <c r="AY10" s="2">
+      <c r="AY10">
         <v>47.6</v>
       </c>
-      <c r="AZ10" s="2">
+      <c r="AZ10">
         <v>18.3</v>
       </c>
-      <c r="BA10" s="2">
+      <c r="BA10">
         <v>34.6</v>
       </c>
-      <c r="BB10" s="2">
+      <c r="BB10">
         <v>0.528</v>
       </c>
-      <c r="BC10" s="2"/>
-      <c r="BD10" s="2"/>
-      <c r="BE10" s="2"/>
-      <c r="BF10" s="2">
+      <c r="BF10">
         <v>18.3</v>
       </c>
-      <c r="BG10" s="2">
+      <c r="BG10">
         <v>34.6</v>
       </c>
-      <c r="BH10" s="2">
+      <c r="BH10">
         <v>0.528</v>
       </c>
-      <c r="BI10" s="2">
+      <c r="BI10">
         <v>0.528</v>
       </c>
-      <c r="BJ10" s="2">
+      <c r="BJ10">
         <v>8.300000000000001</v>
       </c>
-      <c r="BK10" s="2">
+      <c r="BK10">
         <v>13.9</v>
       </c>
-      <c r="BL10" s="2">
+      <c r="BL10">
         <v>0.593</v>
       </c>
-      <c r="BM10" s="2"/>
-      <c r="BN10" s="2"/>
-      <c r="BO10" s="2">
+      <c r="BO10">
         <v>24.3</v>
       </c>
-      <c r="BP10" s="2">
+      <c r="BP10">
         <v>3.4</v>
       </c>
-      <c r="BQ10" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="BR10" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="BS10" s="2"/>
-      <c r="BT10" s="2">
+      <c r="BQ10" t="s">
+        <v>91</v>
+      </c>
+      <c r="BR10" t="s">
+        <v>91</v>
+      </c>
+      <c r="BT10">
         <v>1.7</v>
       </c>
-      <c r="BU10" s="2">
+      <c r="BU10">
         <v>44.8</v>
       </c>
-      <c r="BV10" s="2" t="s">
+      <c r="BV10" t="s">
         <v>98</v>
       </c>
-      <c r="BW10" s="2" t="s">
+      <c r="BW10" t="s">
         <v>103</v>
       </c>
-      <c r="BX10" s="2" t="s">
+      <c r="BX10" t="s">
         <v>102</v>
       </c>
-      <c r="BY10" s="2">
+      <c r="BY10">
         <v>1963</v>
       </c>
     </row>
     <row r="11" spans="1:77">
-      <c r="A11" s="2">
+      <c r="A11">
         <v>2332</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" t="s">
         <v>84</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11">
         <v>610</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" t="s">
         <v>87</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11">
         <v>1935</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" t="s">
         <v>88</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11">
         <v>27</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H11">
         <v>6</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="I11" t="s">
         <v>89</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="J11" t="s">
         <v>90</v>
       </c>
-      <c r="K11" s="2">
+      <c r="K11">
         <v>76</v>
       </c>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2">
+      <c r="M11">
         <v>45.2</v>
       </c>
-      <c r="N11" s="2">
+      <c r="N11">
         <v>7.6</v>
       </c>
-      <c r="O11" s="2">
+      <c r="O11">
         <v>16.6</v>
       </c>
-      <c r="P11" s="2">
+      <c r="P11">
         <v>0.457</v>
       </c>
-      <c r="Q11" s="2"/>
-      <c r="R11" s="2"/>
-      <c r="S11" s="2"/>
-      <c r="T11" s="2">
+      <c r="T11">
         <v>7.6</v>
       </c>
-      <c r="U11" s="2">
+      <c r="U11">
         <v>16.6</v>
       </c>
-      <c r="V11" s="2">
+      <c r="V11">
         <v>0.457</v>
       </c>
-      <c r="W11" s="2">
+      <c r="W11">
         <v>0.457</v>
       </c>
-      <c r="X11" s="2">
+      <c r="X11">
         <v>3.8</v>
       </c>
-      <c r="Y11" s="2">
+      <c r="Y11">
         <v>6.3</v>
       </c>
-      <c r="Z11" s="2">
+      <c r="Z11">
         <v>0.595</v>
       </c>
-      <c r="AA11" s="2"/>
-      <c r="AB11" s="2"/>
-      <c r="AC11" s="2">
+      <c r="AC11">
         <v>23.6</v>
       </c>
-      <c r="AD11" s="2">
+      <c r="AD11">
         <v>4.5</v>
       </c>
-      <c r="AE11" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AF11" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AG11" s="2"/>
-      <c r="AH11" s="2">
+      <c r="AE11" t="s">
+        <v>91</v>
+      </c>
+      <c r="AF11" t="s">
+        <v>91</v>
+      </c>
+      <c r="AH11">
         <v>2.7</v>
       </c>
-      <c r="AI11" s="3">
+      <c r="AI11">
         <v>18.9</v>
       </c>
-      <c r="AJ11" s="2" t="s">
+      <c r="AJ11" t="s">
         <v>99</v>
       </c>
-      <c r="AK11" s="2" t="s">
+      <c r="AK11" t="s">
         <v>103</v>
       </c>
-      <c r="AL11" s="2" t="s">
+      <c r="AL11" t="s">
         <v>102</v>
       </c>
-      <c r="AM11" s="2">
+      <c r="AM11">
         <v>1962</v>
       </c>
-      <c r="AN11" s="2">
+      <c r="AN11">
         <v>2445</v>
       </c>
-      <c r="AO11" s="2">
+      <c r="AO11">
         <v>699</v>
       </c>
-      <c r="AP11" s="2" t="s">
+      <c r="AP11" t="s">
         <v>104</v>
       </c>
-      <c r="AQ11" s="2">
+      <c r="AQ11">
         <v>1937</v>
       </c>
-      <c r="AR11" s="2" t="s">
+      <c r="AR11" t="s">
         <v>88</v>
       </c>
-      <c r="AS11" s="2">
+      <c r="AS11">
         <v>25</v>
       </c>
-      <c r="AT11" s="2">
+      <c r="AT11">
         <v>3</v>
       </c>
-      <c r="AU11" s="2" t="s">
+      <c r="AU11" t="s">
         <v>89</v>
       </c>
-      <c r="AV11" s="2" t="s">
+      <c r="AV11" t="s">
         <v>109</v>
       </c>
-      <c r="AW11" s="2">
+      <c r="AW11">
         <v>80</v>
       </c>
-      <c r="AX11" s="2"/>
-      <c r="AY11" s="2">
+      <c r="AY11">
         <v>48.5</v>
       </c>
-      <c r="AZ11" s="2">
+      <c r="AZ11">
         <v>20</v>
       </c>
-      <c r="BA11" s="2">
+      <c r="BA11">
         <v>39.5</v>
       </c>
-      <c r="BB11" s="2">
+      <c r="BB11">
         <v>0.506</v>
       </c>
-      <c r="BC11" s="2"/>
-      <c r="BD11" s="2"/>
-      <c r="BE11" s="2"/>
-      <c r="BF11" s="2">
+      <c r="BF11">
         <v>20</v>
       </c>
-      <c r="BG11" s="2">
+      <c r="BG11">
         <v>39.5</v>
       </c>
-      <c r="BH11" s="2">
+      <c r="BH11">
         <v>0.506</v>
       </c>
-      <c r="BI11" s="2">
+      <c r="BI11">
         <v>0.506</v>
       </c>
-      <c r="BJ11" s="2">
+      <c r="BJ11">
         <v>10.4</v>
       </c>
-      <c r="BK11" s="2">
+      <c r="BK11">
         <v>17</v>
       </c>
-      <c r="BL11" s="2">
+      <c r="BL11">
         <v>0.613</v>
       </c>
-      <c r="BM11" s="2"/>
-      <c r="BN11" s="2"/>
-      <c r="BO11" s="2">
+      <c r="BO11">
         <v>25.7</v>
       </c>
-      <c r="BP11" s="2">
+      <c r="BP11">
         <v>2.4</v>
       </c>
-      <c r="BQ11" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="BR11" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="BS11" s="2"/>
-      <c r="BT11" s="2">
+      <c r="BQ11" t="s">
+        <v>91</v>
+      </c>
+      <c r="BR11" t="s">
+        <v>91</v>
+      </c>
+      <c r="BT11">
         <v>1.5</v>
       </c>
-      <c r="BU11" s="3">
+      <c r="BU11">
         <v>50.4</v>
       </c>
-      <c r="BV11" s="2" t="s">
+      <c r="BV11" t="s">
         <v>99</v>
       </c>
-      <c r="BW11" s="2" t="s">
+      <c r="BW11" t="s">
         <v>103</v>
       </c>
-      <c r="BX11" s="2" t="s">
+      <c r="BX11" t="s">
         <v>102</v>
       </c>
-      <c r="BY11" s="2">
+      <c r="BY11">
         <v>1962</v>
       </c>
     </row>
     <row r="12" spans="1:77">
-      <c r="A12" s="2">
+      <c r="A12">
         <v>2219</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" t="s">
         <v>85</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12">
         <v>610</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" t="s">
         <v>87</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12">
         <v>1935</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" t="s">
         <v>88</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G12">
         <v>26</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H12">
         <v>5</v>
       </c>
-      <c r="I12" s="2" t="s">
+      <c r="I12" t="s">
         <v>89</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="J12" t="s">
         <v>90</v>
       </c>
-      <c r="K12" s="2">
+      <c r="K12">
         <v>78</v>
       </c>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2">
+      <c r="M12">
         <v>44.3</v>
       </c>
-      <c r="N12" s="2">
+      <c r="N12">
         <v>6.8</v>
       </c>
-      <c r="O12" s="2">
+      <c r="O12">
         <v>16</v>
       </c>
-      <c r="P12" s="2">
+      <c r="P12">
         <v>0.426</v>
       </c>
-      <c r="Q12" s="2"/>
-      <c r="R12" s="2"/>
-      <c r="S12" s="2"/>
-      <c r="T12" s="2">
+      <c r="T12">
         <v>6.8</v>
       </c>
-      <c r="U12" s="2">
+      <c r="U12">
         <v>16</v>
       </c>
-      <c r="V12" s="2">
+      <c r="V12">
         <v>0.426</v>
       </c>
-      <c r="W12" s="2">
+      <c r="W12">
         <v>0.426</v>
       </c>
-      <c r="X12" s="2">
+      <c r="X12">
         <v>3.3</v>
       </c>
-      <c r="Y12" s="2">
+      <c r="Y12">
         <v>6</v>
       </c>
-      <c r="Z12" s="2">
+      <c r="Z12">
         <v>0.55</v>
       </c>
-      <c r="AA12" s="2"/>
-      <c r="AB12" s="2"/>
-      <c r="AC12" s="2">
+      <c r="AC12">
         <v>23.9</v>
       </c>
-      <c r="AD12" s="2">
+      <c r="AD12">
         <v>3.4</v>
       </c>
-      <c r="AE12" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AF12" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AG12" s="2"/>
-      <c r="AH12" s="2">
+      <c r="AE12" t="s">
+        <v>91</v>
+      </c>
+      <c r="AF12" t="s">
+        <v>91</v>
+      </c>
+      <c r="AH12">
         <v>2</v>
       </c>
-      <c r="AI12" s="2">
+      <c r="AI12">
         <v>16.9</v>
       </c>
-      <c r="AJ12" s="2" t="s">
+      <c r="AJ12" t="s">
         <v>100</v>
       </c>
-      <c r="AK12" s="2" t="s">
+      <c r="AK12" t="s">
         <v>103</v>
       </c>
-      <c r="AL12" s="2" t="s">
+      <c r="AL12" t="s">
         <v>102</v>
       </c>
-      <c r="AM12" s="2">
+      <c r="AM12">
         <v>1961</v>
       </c>
-      <c r="AN12" s="2">
+      <c r="AN12">
         <v>2313</v>
       </c>
-      <c r="AO12" s="2">
+      <c r="AO12">
         <v>699</v>
       </c>
-      <c r="AP12" s="2" t="s">
+      <c r="AP12" t="s">
         <v>104</v>
       </c>
-      <c r="AQ12" s="2">
+      <c r="AQ12">
         <v>1937</v>
       </c>
-      <c r="AR12" s="2" t="s">
+      <c r="AR12" t="s">
         <v>88</v>
       </c>
-      <c r="AS12" s="2">
+      <c r="AS12">
         <v>24</v>
       </c>
-      <c r="AT12" s="2">
+      <c r="AT12">
         <v>2</v>
       </c>
-      <c r="AU12" s="2" t="s">
+      <c r="AU12" t="s">
         <v>89</v>
       </c>
-      <c r="AV12" s="2" t="s">
+      <c r="AV12" t="s">
         <v>109</v>
       </c>
-      <c r="AW12" s="2">
+      <c r="AW12">
         <v>79</v>
       </c>
-      <c r="AX12" s="2"/>
-      <c r="AY12" s="2">
+      <c r="AY12">
         <v>47.8</v>
       </c>
-      <c r="AZ12" s="2">
+      <c r="AZ12">
         <v>15.8</v>
       </c>
-      <c r="BA12" s="2">
+      <c r="BA12">
         <v>31.1</v>
       </c>
-      <c r="BB12" s="2">
+      <c r="BB12">
         <v>0.509</v>
       </c>
-      <c r="BC12" s="2"/>
-      <c r="BD12" s="2"/>
-      <c r="BE12" s="2"/>
-      <c r="BF12" s="2">
+      <c r="BF12">
         <v>15.8</v>
       </c>
-      <c r="BG12" s="2">
+      <c r="BG12">
         <v>31.1</v>
       </c>
-      <c r="BH12" s="2">
+      <c r="BH12">
         <v>0.509</v>
       </c>
-      <c r="BI12" s="2">
+      <c r="BI12">
         <v>0.509</v>
       </c>
-      <c r="BJ12" s="2">
+      <c r="BJ12">
         <v>6.7</v>
       </c>
-      <c r="BK12" s="2">
+      <c r="BK12">
         <v>13.3</v>
       </c>
-      <c r="BL12" s="2">
+      <c r="BL12">
         <v>0.504</v>
       </c>
-      <c r="BM12" s="2"/>
-      <c r="BN12" s="2"/>
-      <c r="BO12" s="3">
+      <c r="BO12">
         <v>27.2</v>
       </c>
-      <c r="BP12" s="2">
+      <c r="BP12">
         <v>1.9</v>
       </c>
-      <c r="BQ12" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="BR12" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="BS12" s="2"/>
-      <c r="BT12" s="2">
+      <c r="BQ12" t="s">
+        <v>91</v>
+      </c>
+      <c r="BR12" t="s">
+        <v>91</v>
+      </c>
+      <c r="BT12">
         <v>1.6</v>
       </c>
-      <c r="BU12" s="2">
+      <c r="BU12">
         <v>38.4</v>
       </c>
-      <c r="BV12" s="2" t="s">
+      <c r="BV12" t="s">
         <v>100</v>
       </c>
-      <c r="BW12" s="2" t="s">
+      <c r="BW12" t="s">
         <v>103</v>
       </c>
-      <c r="BX12" s="2" t="s">
+      <c r="BX12" t="s">
         <v>102</v>
       </c>
-      <c r="BY12" s="2">
+      <c r="BY12">
         <v>1961</v>
       </c>
     </row>
     <row r="13" spans="1:77">
-      <c r="A13" s="2">
+      <c r="A13">
         <v>2097</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" t="s">
         <v>86</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13">
         <v>610</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" t="s">
         <v>87</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13">
         <v>1935</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" t="s">
         <v>88</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G13">
         <v>25</v>
       </c>
-      <c r="H13" s="2">
+      <c r="H13">
         <v>4</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="I13" t="s">
         <v>89</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="J13" t="s">
         <v>90</v>
       </c>
-      <c r="K13" s="2">
+      <c r="K13">
         <v>74</v>
       </c>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2">
+      <c r="M13">
         <v>42.5</v>
       </c>
-      <c r="N13" s="2">
+      <c r="N13">
         <v>7.5</v>
       </c>
-      <c r="O13" s="2">
+      <c r="O13">
         <v>16.1</v>
       </c>
-      <c r="P13" s="2">
+      <c r="P13">
         <v>0.467</v>
       </c>
-      <c r="Q13" s="2"/>
-      <c r="R13" s="2"/>
-      <c r="S13" s="2"/>
-      <c r="T13" s="2">
+      <c r="T13">
         <v>7.5</v>
       </c>
-      <c r="U13" s="2">
+      <c r="U13">
         <v>16.1</v>
       </c>
-      <c r="V13" s="2">
+      <c r="V13">
         <v>0.467</v>
       </c>
-      <c r="W13" s="2">
+      <c r="W13">
         <v>0.467</v>
       </c>
-      <c r="X13" s="2">
+      <c r="X13">
         <v>3.2</v>
       </c>
-      <c r="Y13" s="2">
+      <c r="Y13">
         <v>5.3</v>
       </c>
-      <c r="Z13" s="2">
+      <c r="Z13">
         <v>0.612</v>
       </c>
-      <c r="AA13" s="2"/>
-      <c r="AB13" s="2"/>
-      <c r="AC13" s="2">
+      <c r="AC13">
         <v>24</v>
       </c>
-      <c r="AD13" s="2">
+      <c r="AD13">
         <v>3.7</v>
       </c>
-      <c r="AE13" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AF13" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AG13" s="2"/>
-      <c r="AH13" s="2">
+      <c r="AE13" t="s">
+        <v>91</v>
+      </c>
+      <c r="AF13" t="s">
+        <v>91</v>
+      </c>
+      <c r="AH13">
         <v>2.8</v>
       </c>
-      <c r="AI13" s="2">
+      <c r="AI13">
         <v>18.2</v>
       </c>
-      <c r="AJ13" s="2" t="s">
+      <c r="AJ13" t="s">
         <v>101</v>
       </c>
-      <c r="AK13" s="2" t="s">
+      <c r="AK13" t="s">
         <v>103</v>
       </c>
-      <c r="AL13" s="2" t="s">
+      <c r="AL13" t="s">
         <v>102</v>
       </c>
-      <c r="AM13" s="2">
+      <c r="AM13">
         <v>1960</v>
       </c>
-      <c r="AN13" s="2">
+      <c r="AN13">
         <v>2209</v>
       </c>
-      <c r="AO13" s="2">
+      <c r="AO13">
         <v>699</v>
       </c>
-      <c r="AP13" s="2" t="s">
+      <c r="AP13" t="s">
         <v>104</v>
       </c>
-      <c r="AQ13" s="2">
+      <c r="AQ13">
         <v>1937</v>
       </c>
-      <c r="AR13" s="2" t="s">
+      <c r="AR13" t="s">
         <v>88</v>
       </c>
-      <c r="AS13" s="2">
+      <c r="AS13">
         <v>23</v>
       </c>
-      <c r="AT13" s="2">
+      <c r="AT13">
         <v>1</v>
       </c>
-      <c r="AU13" s="2" t="s">
+      <c r="AU13" t="s">
         <v>89</v>
       </c>
-      <c r="AV13" s="2" t="s">
+      <c r="AV13" t="s">
         <v>109</v>
       </c>
-      <c r="AW13" s="2">
+      <c r="AW13">
         <v>72</v>
       </c>
-      <c r="AX13" s="2"/>
-      <c r="AY13" s="2">
+      <c r="AY13">
         <v>46.4</v>
       </c>
-      <c r="AZ13" s="2">
+      <c r="AZ13">
         <v>14.8</v>
       </c>
-      <c r="BA13" s="2">
+      <c r="BA13">
         <v>32.1</v>
       </c>
-      <c r="BB13" s="2">
+      <c r="BB13">
         <v>0.461</v>
       </c>
-      <c r="BC13" s="2"/>
-      <c r="BD13" s="2"/>
-      <c r="BE13" s="2"/>
-      <c r="BF13" s="2">
+      <c r="BF13">
         <v>14.8</v>
       </c>
-      <c r="BG13" s="2">
+      <c r="BG13">
         <v>32.1</v>
       </c>
-      <c r="BH13" s="2">
+      <c r="BH13">
         <v>0.461</v>
       </c>
-      <c r="BI13" s="2">
+      <c r="BI13">
         <v>0.461</v>
       </c>
-      <c r="BJ13" s="2">
+      <c r="BJ13">
         <v>8</v>
       </c>
-      <c r="BK13" s="2">
+      <c r="BK13">
         <v>13.8</v>
       </c>
-      <c r="BL13" s="2">
+      <c r="BL13">
         <v>0.582</v>
       </c>
-      <c r="BM13" s="2"/>
-      <c r="BN13" s="2"/>
-      <c r="BO13" s="2">
+      <c r="BO13">
         <v>27</v>
       </c>
-      <c r="BP13" s="2">
+      <c r="BP13">
         <v>2.3</v>
       </c>
-      <c r="BQ13" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="BR13" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="BS13" s="2"/>
-      <c r="BT13" s="2">
+      <c r="BQ13" t="s">
+        <v>91</v>
+      </c>
+      <c r="BR13" t="s">
+        <v>91</v>
+      </c>
+      <c r="BT13">
         <v>2.1</v>
       </c>
-      <c r="BU13" s="2">
+      <c r="BU13">
         <v>37.6</v>
       </c>
-      <c r="BV13" s="2" t="s">
+      <c r="BV13" t="s">
         <v>101</v>
       </c>
-      <c r="BW13" s="2" t="s">
+      <c r="BW13" t="s">
         <v>103</v>
       </c>
-      <c r="BX13" s="2" t="s">
+      <c r="BX13" t="s">
         <v>102</v>
       </c>
-      <c r="BY13" s="2">
+      <c r="BY13">
         <v>1960</v>
       </c>
     </row>

</xml_diff>